<commit_message>
Materia logic - second changes
</commit_message>
<xml_diff>
--- a/definitions/material.xlsx
+++ b/definitions/material.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="238">
   <si>
     <t>TABLE_NAME</t>
   </si>
@@ -46,12 +46,18 @@
     <t>generate_product_number()</t>
   </si>
   <si>
+    <t>This function generates product numbers following patterns that we have already identified based on the material preload file.</t>
+  </si>
+  <si>
     <t>MTART</t>
   </si>
   <si>
     <t>assign_product_type(PRODUCT)</t>
   </si>
   <si>
+    <t>The assing_product_type function sets the product type according to the rules in the mapping-rule column. It takes the generated product number and assigns the corresponding product type based on how that ID was created.</t>
+  </si>
+  <si>
     <t>MATKL</t>
   </si>
   <si>
@@ -64,6 +70,9 @@
     <t>default_value("M")</t>
   </si>
   <si>
+    <t>The default function generates a default value based on the one the user assigns as a parameter.</t>
+  </si>
+  <si>
     <t>MAKTX</t>
   </si>
   <si>
@@ -91,6 +100,9 @@
     <t>old_product_id()</t>
   </si>
   <si>
+    <t>The old_product_id function generates a fake old product number based on the patterns identified in the material preload sample data.</t>
+  </si>
+  <si>
     <t>PRDHA</t>
   </si>
   <si>
@@ -178,6 +190,9 @@
     <t>get_datetime()</t>
   </si>
   <si>
+    <t>The get_datetime function returns the current date.</t>
+  </si>
+  <si>
     <t>SOM_CYCLE</t>
   </si>
   <si>
@@ -259,6 +274,9 @@
     <t>fk_copy("S_MAKT")</t>
   </si>
   <si>
+    <t>This function simulates a similar one‑to‑one FK relationship.</t>
+  </si>
+  <si>
     <t xml:space="preserve">40    </t>
   </si>
   <si>
@@ -292,6 +310,9 @@
     <t>get_random_grouping_terms()</t>
   </si>
   <si>
+    <t>The function assigns a random grouping term based on those defined in the mapping file.</t>
+  </si>
+  <si>
     <t>SKTOF</t>
   </si>
   <si>
@@ -331,6 +352,9 @@
     <t>get_random_distribution_channels()</t>
   </si>
   <si>
+    <t>The function assigns a random distribution channel based on those defined in the mapping file.</t>
+  </si>
+  <si>
     <t>VMSTA</t>
   </si>
   <si>
@@ -355,6 +379,9 @@
     <t>get_sales_org(DWERK)</t>
   </si>
   <si>
+    <t>The function assigns the Sales Org value based on the value assigned in the Delivery Plant column.</t>
+  </si>
+  <si>
     <t>VRKME</t>
   </si>
   <si>
@@ -382,12 +409,18 @@
     <t>get_country("S_MVKE", "PRODUCT","DWERK",PRODUCT)</t>
   </si>
   <si>
+    <t>The get_country function uses the lookup_parent_value function to look up the value assigned to a product number in the parent S_MVKE table, using the Delivery Plant as a reference, and based on the returned value, it assigns a country value.</t>
+  </si>
+  <si>
     <t>TATYP1</t>
   </si>
   <si>
     <t>get_sales_tax_cat_one(ALAND)</t>
   </si>
   <si>
+    <t>The function assigns the Sales Tax Category value based on the value assigned in the Country column.</t>
+  </si>
+  <si>
     <t>TAXM1</t>
   </si>
   <si>
@@ -403,6 +436,9 @@
     <t>lookup_parent_value("S_MVKE", "PRODUCT","DWERK",PRODUCT)</t>
   </si>
   <si>
+    <t>The function looks up the value assigned to a product number using the Delivery Plant as a reference in the parent S_MVKE table.</t>
+  </si>
+  <si>
     <t>DISMM</t>
   </si>
   <si>
@@ -514,6 +550,10 @@
     <t>fk_copy("S_MLGN")</t>
   </si>
   <si>
+    <t xml:space="preserve">This function simulates a similar one‑to‑one FK relationship.
+</t>
+  </si>
+  <si>
     <t>S_MLGT</t>
   </si>
   <si>
@@ -541,6 +581,9 @@
     <t>get_valuation_class("S_MARA", "PRODUCT","MTART",PRODUCT)</t>
   </si>
   <si>
+    <t>The get_valuation_class function uses the lookup_parent_value function to look up the value assigned to a product number in the parent S_MVKE table, using the Delivery Plant as a reference, and based on the returned value, it assigns a valuation class.</t>
+  </si>
+  <si>
     <t>VPRSV</t>
   </si>
   <si>
@@ -551,6 +594,9 @@
   </si>
   <si>
     <t>get_currency("S_MVKE", "PRODUCT","DWERK",PRODUCT)</t>
+  </si>
+  <si>
+    <t>The get_currency function uses the lookup_parent_value function to look up the value assigned to a product number in the parent S_MVKE table, using the Delivery Plant as a reference, and based on the returned value, it assigns a currency value.</t>
   </si>
   <si>
     <t>VERPR</t>
@@ -639,6 +685,51 @@
   </si>
   <si>
     <t>ZPRSDAT_1</t>
+  </si>
+  <si>
+    <t>SAPAPO_MATLSP</t>
+  </si>
+  <si>
+    <t>BUY_PLNR</t>
+  </si>
+  <si>
+    <t>default_value("SPP")</t>
+  </si>
+  <si>
+    <t>FCS_PLNR</t>
+  </si>
+  <si>
+    <t>SCA_PLNR</t>
+  </si>
+  <si>
+    <t>DRP_PLNR</t>
+  </si>
+  <si>
+    <t>IPL_PLNR</t>
+  </si>
+  <si>
+    <t>REPLINDI</t>
+  </si>
+  <si>
+    <t>default_value("ST")</t>
+  </si>
+  <si>
+    <t>PROC_TO_ORD</t>
+  </si>
+  <si>
+    <t>DRP_PLAN_MODE</t>
+  </si>
+  <si>
+    <t>MARC</t>
+  </si>
+  <si>
+    <t>SCM_PROC_COST</t>
+  </si>
+  <si>
+    <t>SCM_SCOST_PRCNT</t>
+  </si>
+  <si>
+    <t>default_value("0.20")</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1095,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F160"/>
+  <dimension ref="A1:F158"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1014,11 +1105,11 @@
     <col min="2" max="2" style="3" width="18.005" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="4" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="35.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="59.86214285714286" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="3" width="51.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25" hidden="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25" hidden="1">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1054,14 +1145,16 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25" hidden="1">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -1070,16 +1163,18 @@
         <v>80</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -1089,15 +1184,15 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25" hidden="1">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -1106,16 +1201,18 @@
         <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -1125,15 +1222,15 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25" hidden="1">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -1142,16 +1239,18 @@
         <v>80</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25" hidden="1">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>8</v>
@@ -1160,16 +1259,18 @@
         <v>80</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25" hidden="1">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
@@ -1178,16 +1279,18 @@
         <v>80</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+        <v>25</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25" hidden="1">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
@@ -1196,16 +1299,18 @@
         <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
@@ -1215,15 +1320,15 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25" hidden="1">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
@@ -1232,16 +1337,18 @@
         <v>80</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
@@ -1251,7 +1358,7 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
@@ -1259,17 +1366,17 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2">
         <v>13</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
@@ -1277,17 +1384,17 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2">
         <v>13</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
@@ -1295,7 +1402,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>8</v>
@@ -1305,7 +1412,7 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
@@ -1313,17 +1420,17 @@
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D17" s="2">
         <v>13</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
@@ -1331,17 +1438,17 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D18" s="2">
         <v>13</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
@@ -1349,17 +1456,17 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D19" s="2">
         <v>3</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
@@ -1367,7 +1474,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
@@ -1377,7 +1484,7 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
@@ -1385,17 +1492,17 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D21" s="2">
         <v>13</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
@@ -1403,7 +1510,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>8</v>
@@ -1413,7 +1520,7 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
@@ -1421,7 +1528,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>8</v>
@@ -1431,15 +1538,15 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
+        <v>46</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25" hidden="1">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>8</v>
@@ -1448,16 +1555,18 @@
         <v>80</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
+        <v>23</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25" hidden="1">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>8</v>
@@ -1466,16 +1575,18 @@
         <v>80</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>8</v>
@@ -1485,15 +1596,15 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
+        <v>51</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25" hidden="1">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>8</v>
@@ -1502,16 +1613,18 @@
         <v>80</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>8</v>
@@ -1521,31 +1634,33 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25" hidden="1">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
+        <v>57</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25" hidden="1">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>8</v>
@@ -1554,16 +1669,18 @@
         <v>80</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>8</v>
@@ -1573,7 +1690,7 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
@@ -1581,17 +1698,17 @@
         <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D32" s="2">
         <v>13</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
@@ -1599,7 +1716,7 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>8</v>
@@ -1609,7 +1726,7 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
@@ -1617,17 +1734,17 @@
         <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D34" s="2">
         <v>3</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
@@ -1635,17 +1752,17 @@
         <v>6</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D35" s="2">
         <v>3</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
@@ -1653,7 +1770,7 @@
         <v>6</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>8</v>
@@ -1663,7 +1780,7 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
@@ -1671,25 +1788,25 @@
         <v>6</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D37" s="2">
         <v>3</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25" hidden="1">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>8</v>
@@ -1698,16 +1815,18 @@
         <v>80</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F38" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
@@ -1717,7 +1836,7 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
@@ -1725,7 +1844,7 @@
         <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
@@ -1735,7 +1854,7 @@
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
@@ -1743,7 +1862,7 @@
         <v>6</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>8</v>
@@ -1753,7 +1872,7 @@
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
@@ -1761,7 +1880,7 @@
         <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>8</v>
@@ -1771,7 +1890,7 @@
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
@@ -1779,25 +1898,25 @@
         <v>6</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D43" s="2">
         <v>4</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
+        <v>75</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25" hidden="1">
       <c r="A44" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>8</v>
@@ -1806,16 +1925,18 @@
         <v>80</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F44" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
@@ -1825,15 +1946,15 @@
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25" hidden="1">
       <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>8</v>
@@ -1842,16 +1963,18 @@
         <v>80</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F46" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18">
       <c r="A47" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>8</v>
@@ -1861,7 +1984,7 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18">
@@ -1869,7 +1992,7 @@
         <v>6</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>8</v>
@@ -1879,12 +2002,12 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25" hidden="1">
       <c r="A49" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>7</v>
@@ -1893,52 +2016,56 @@
         <v>8</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F49" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18">
+        <v>85</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25" hidden="1">
       <c r="A50" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F50" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18">
       <c r="A51" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25" hidden="1">
       <c r="A52" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>7</v>
@@ -1946,55 +2073,57 @@
       <c r="C52" s="1"/>
       <c r="D52" s="2"/>
       <c r="E52" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F52" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18">
       <c r="A53" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="2"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18">
       <c r="A54" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="2"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18">
       <c r="A55" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="2"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25" hidden="1">
       <c r="A56" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>7</v>
@@ -2003,214 +2132,232 @@
         <v>8</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F56" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18">
+        <v>94</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25" hidden="1">
       <c r="A57" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F57" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18">
+        <v>97</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25" hidden="1">
       <c r="A58" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F58" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18">
+        <v>101</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25" hidden="1">
       <c r="A59" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25" hidden="1">
+      <c r="A60" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F59" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18">
-      <c r="A60" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="B60" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F60" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18">
+        <v>104</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25" hidden="1">
       <c r="A61" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F61" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18">
       <c r="A62" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25" hidden="1">
       <c r="A63" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F63" s="1"/>
+        <v>111</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18">
       <c r="A64" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25" hidden="1">
       <c r="A65" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F65" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18">
+        <v>115</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25" hidden="1">
       <c r="A66" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F66" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18">
       <c r="A67" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="17.25" hidden="1">
       <c r="A68" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>7</v>
@@ -2219,122 +2366,136 @@
         <v>8</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F68" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18">
+        <v>118</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="17.25" hidden="1">
       <c r="A69" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F69" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18">
+        <v>120</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="17.25" hidden="1">
       <c r="A70" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F70" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18">
+        <v>23</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="17.25" hidden="1">
       <c r="A71" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F71" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18">
+        <v>17</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="17.25" hidden="1">
       <c r="A72" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F72" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18">
+        <v>17</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="17.25" hidden="1">
       <c r="A73" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F73" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18">
+        <v>23</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="17.25" hidden="1">
       <c r="A74" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F74" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18">
+        <v>57</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="17.25" hidden="1">
       <c r="A75" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>7</v>
@@ -2343,70 +2504,78 @@
         <v>8</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F75" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18">
+        <v>128</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="17.25" hidden="1">
       <c r="A76" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F76" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18">
+        <v>130</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="17.25" hidden="1">
       <c r="A77" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F77" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18">
+        <v>133</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="17.25" hidden="1">
       <c r="A78" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F78" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18">
+        <v>49</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="17.25" hidden="1">
       <c r="A79" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>7</v>
@@ -2415,340 +2584,358 @@
         <v>8</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F79" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18">
+        <v>137</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="17.25" hidden="1">
       <c r="A80" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F80" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18">
+        <v>139</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="17.25" hidden="1">
       <c r="A81" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F81" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18">
       <c r="A82" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="17.25" hidden="1">
       <c r="A83" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F83" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18">
       <c r="A84" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="17.25" hidden="1">
       <c r="A85" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F85" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18">
       <c r="A86" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18">
+        <v>51</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="17.25" hidden="1">
       <c r="A87" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F87" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18">
       <c r="A88" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18">
       <c r="A89" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18">
+        <v>51</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="17.25" hidden="1">
       <c r="A90" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F90" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18">
+        <v>101</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="17.25" hidden="1">
       <c r="A91" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F91" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18">
+        <v>49</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="17.25" hidden="1">
       <c r="A92" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F92" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18">
       <c r="A93" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18">
       <c r="A94" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18">
       <c r="A95" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18">
       <c r="A96" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18">
       <c r="A97" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="17.25" hidden="1">
       <c r="A98" s="1" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>7</v>
@@ -2757,52 +2944,56 @@
         <v>8</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F98" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18">
+        <v>163</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="17.25" hidden="1">
       <c r="A99" s="1" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F99" s="1"/>
+        <v>139</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18">
       <c r="A100" s="1" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18">
+        <v>165</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="17.25" hidden="1">
       <c r="A101" s="1" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>7</v>
@@ -2811,160 +3002,168 @@
         <v>8</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F101" s="1"/>
+        <v>167</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18">
       <c r="A102" s="1" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18">
+        <v>169</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="17.25" hidden="1">
       <c r="A103" s="1" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F103" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18">
+        <v>139</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="17.25" hidden="1">
       <c r="A104" s="1" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F104" s="1"/>
+        <v>170</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18">
       <c r="A105" s="1" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="17.25" hidden="1">
       <c r="A106" s="1" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F106" s="1"/>
+        <v>172</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18">
       <c r="A107" s="1" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18">
       <c r="A108" s="1" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18">
       <c r="A109" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="C109" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18">
+        <v>175</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="17.25" hidden="1">
       <c r="A110" s="1" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>7</v>
@@ -2973,16 +3172,18 @@
         <v>8</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F110" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18">
+        <v>177</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="17.25" hidden="1">
       <c r="A111" s="1" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>7</v>
@@ -2991,16 +3192,18 @@
         <v>8</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F111" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18">
+        <v>180</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="17.25" hidden="1">
       <c r="A112" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>7</v>
@@ -3009,404 +3212,416 @@
         <v>8</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F112" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18">
+        <v>182</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="17.25" hidden="1">
       <c r="A113" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F113" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18">
+        <v>139</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="17.25" hidden="1">
       <c r="A114" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F114" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18">
+        <v>185</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="17.25" hidden="1">
       <c r="A115" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F115" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18">
+        <v>187</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="17.25" hidden="1">
       <c r="A116" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F116" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18">
+        <v>190</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="17.25" hidden="1">
       <c r="A117" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F117" s="1"/>
+        <v>192</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18">
       <c r="A118" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18">
       <c r="A119" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18">
       <c r="A120" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18">
       <c r="A121" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D121" s="2"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18">
       <c r="A122" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18">
       <c r="A123" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D123" s="2"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18">
       <c r="A124" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18">
       <c r="A125" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D125" s="2"/>
       <c r="E125" s="1"/>
       <c r="F125" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18">
       <c r="A126" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18">
       <c r="A127" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D127" s="2"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18">
       <c r="A128" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18">
       <c r="A129" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
       <c r="A130" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B130" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D130" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D130" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
       <c r="A131" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
       <c r="A132" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
       <c r="A133" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
       <c r="A134" s="1" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
+        <v>199</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="17.25" hidden="1">
       <c r="A135" s="1" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>7</v>
@@ -3415,124 +3630,134 @@
         <v>8</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F135" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
+        <v>216</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="17.25" hidden="1">
       <c r="A136" s="1" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F136" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
+        <v>187</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="17.25" hidden="1">
       <c r="A137" s="1" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F137" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
+        <v>218</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="17.25" hidden="1">
       <c r="A138" s="1" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F138" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
+        <v>190</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="17.25" hidden="1">
       <c r="A139" s="1" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F139" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
+        <v>192</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="19.5">
       <c r="A140" s="1" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
+        <v>199</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="19.5">
       <c r="A141" s="1" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
+        <v>199</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="17.25" hidden="1">
       <c r="A142" s="1" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>7</v>
@@ -3541,214 +3766,324 @@
         <v>8</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F142" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
+        <v>220</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="17.25" hidden="1">
       <c r="A143" s="1" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F143" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
+        <v>187</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="17.25" hidden="1">
       <c r="A144" s="1" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F144" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
+        <v>218</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="17.25" hidden="1">
       <c r="A145" s="1" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F145" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
+        <v>192</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="19.5">
       <c r="A146" s="1" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E146" s="1"/>
       <c r="F146" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
+        <v>199</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="19.5">
       <c r="A147" s="1" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D147" s="2"/>
       <c r="E147" s="1"/>
       <c r="F147" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
+        <v>199</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="19.5">
       <c r="A148" s="1" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="E148" s="1"/>
       <c r="F148" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
-      <c r="A149" s="1"/>
-      <c r="B149" s="1"/>
-      <c r="C149" s="1"/>
-      <c r="D149" s="2"/>
-      <c r="E149" s="1"/>
-      <c r="F149" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
-      <c r="A150" s="1"/>
-      <c r="B150" s="1"/>
-      <c r="C150" s="1"/>
-      <c r="D150" s="2"/>
-      <c r="E150" s="1"/>
-      <c r="F150" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
-      <c r="A151" s="1"/>
-      <c r="B151" s="1"/>
-      <c r="C151" s="1"/>
-      <c r="D151" s="2"/>
-      <c r="E151" s="1"/>
-      <c r="F151" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18">
-      <c r="A152" s="1"/>
-      <c r="B152" s="1"/>
-      <c r="C152" s="1"/>
-      <c r="D152" s="2"/>
-      <c r="E152" s="1"/>
-      <c r="F152" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18">
-      <c r="A153" s="1"/>
-      <c r="B153" s="1"/>
-      <c r="C153" s="1"/>
-      <c r="D153" s="2"/>
-      <c r="E153" s="1"/>
-      <c r="F153" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18">
-      <c r="A154" s="1"/>
-      <c r="B154" s="1"/>
-      <c r="C154" s="1"/>
-      <c r="D154" s="2"/>
-      <c r="E154" s="1"/>
-      <c r="F154" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18">
-      <c r="A155" s="1"/>
-      <c r="B155" s="1"/>
-      <c r="C155" s="1"/>
-      <c r="D155" s="2"/>
-      <c r="E155" s="1"/>
-      <c r="F155" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18">
-      <c r="A156" s="1"/>
-      <c r="B156" s="1"/>
-      <c r="C156" s="1"/>
-      <c r="D156" s="2"/>
-      <c r="E156" s="1"/>
-      <c r="F156" s="1"/>
+        <v>199</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="17.25" hidden="1">
+      <c r="A149" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="17.25" hidden="1">
+      <c r="A150" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="17.25" hidden="1">
+      <c r="A151" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="17.25" hidden="1">
+      <c r="A152" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="17.25" hidden="1">
+      <c r="A153" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="17.25" hidden="1">
+      <c r="A154" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="17.25" hidden="1">
+      <c r="A155" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="17.25" hidden="1">
+      <c r="A156" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18">
-      <c r="A157" s="1"/>
-      <c r="B157" s="1"/>
-      <c r="C157" s="1"/>
-      <c r="D157" s="2"/>
+      <c r="A157" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="E157" s="1"/>
-      <c r="F157" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18">
-      <c r="A158" s="1"/>
-      <c r="B158" s="1"/>
-      <c r="C158" s="1"/>
-      <c r="D158" s="2"/>
-      <c r="E158" s="1"/>
-      <c r="F158" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18">
-      <c r="A159" s="1"/>
-      <c r="B159" s="1"/>
-      <c r="C159" s="1"/>
-      <c r="D159" s="2"/>
-      <c r="E159" s="1"/>
-      <c r="F159" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5">
-      <c r="A160" s="1"/>
-      <c r="B160" s="1"/>
-      <c r="C160" s="1"/>
-      <c r="D160" s="2"/>
-      <c r="E160" s="1"/>
-      <c r="F160" s="1"/>
+      <c r="F157" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="17.25" hidden="1">
+      <c r="A158" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working on the generators doc
</commit_message>
<xml_diff>
--- a/definitions/material.xlsx
+++ b/definitions/material.xlsx
@@ -529,7 +529,7 @@
     <t>HERKL</t>
   </si>
   <si>
-    <t>assing_country_origin(WERKS)</t>
+    <t>assign_country_origin(WERKS)</t>
   </si>
   <si>
     <t>The function assigns a country region.</t>
@@ -1180,7 +1180,7 @@
     <col min="6" max="6" style="3" width="51.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>